<commit_message>
Vérification de l'email fonctionnel
</commit_message>
<xml_diff>
--- a/annexes/Planification.xlsx
+++ b/annexes/Planification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -209,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,12 +235,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -485,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -535,69 +529,62 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="49">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -667,22 +654,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD6E3BC"/>
-          <bgColor rgb="FFD6E3BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBD4B4"/>
-          <bgColor rgb="FFFBD4B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1219,59 +1190,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.125" style="37" customWidth="1"/>
+    <col min="1" max="1" width="73.125" style="35" customWidth="1"/>
     <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="13" width="10.125" customWidth="1"/>
     <col min="14" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="N1" s="41" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="5"/>
@@ -1288,744 +1259,744 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="36">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="46">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="46">
+      <c r="D2" s="47"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="43">
         <f t="shared" ref="N2:N28" si="0">SUM(C2:M2)</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="45">
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="46">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="46">
+      <c r="C3" s="43">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="43">
         <f>SUM(C3:M3)</f>
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="50">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="52">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="46">
+      <c r="D4" s="43"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="43">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="53">
+      <c r="B5" s="50">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="52">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="46">
+      <c r="E5" s="52"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="43">
         <f>SUM(D5:M5)</f>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="50">
         <v>6.25E-2</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="46">
+      <c r="C6" s="52"/>
+      <c r="D6" s="43">
         <v>6.25E-2</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="46">
+      <c r="E6" s="52"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="43">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="50">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="F7" s="46">
+      <c r="C7" s="52"/>
+      <c r="F7" s="43">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="46">
+      <c r="G7" s="52"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="43">
         <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="53">
+      <c r="B8" s="50">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="46">
+      <c r="C8" s="52"/>
+      <c r="D8" s="43">
         <v>0.10416666666666667</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="46">
+      <c r="E8" s="54"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="43">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="50">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="46">
+      <c r="C9" s="52"/>
+      <c r="D9" s="43">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="46">
+      <c r="E9" s="52"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="43">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="50">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="55">
+      <c r="C10" s="54"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="52">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="46">
+      <c r="F10" s="43"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="43">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="53">
+      <c r="B11" s="50">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="55">
+      <c r="C11" s="54"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="52">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="46">
+      <c r="F11" s="43"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="43">
         <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="53">
+      <c r="B12" s="50">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="46">
+      <c r="C12" s="54"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="43">
         <v>0.10416666666666667</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="46">
+      <c r="H12" s="43"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="43">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="53">
+      <c r="B13" s="50">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="46">
+      <c r="C13" s="54"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="43">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H13" s="46"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="46">
+      <c r="H13" s="43"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="43">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="53">
+      <c r="B14" s="50">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="55"/>
-      <c r="G14" s="46">
+      <c r="C14" s="54"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="52"/>
+      <c r="G14" s="43">
         <v>0.10416666666666667</v>
       </c>
-      <c r="H14" s="46"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="46">
+      <c r="H14" s="43"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="43">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="53">
+      <c r="B15" s="50">
         <v>0.125</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="46"/>
-      <c r="H15" s="55">
+      <c r="C15" s="54"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="43"/>
+      <c r="H15" s="52">
         <v>0.125</v>
       </c>
-      <c r="I15" s="57"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="46">
+      <c r="I15" s="54"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="43">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="53">
+      <c r="B16" s="50">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="46"/>
-      <c r="H16" s="55">
+      <c r="C16" s="52"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="43"/>
+      <c r="H16" s="52">
         <v>0.10416666666666667</v>
       </c>
-      <c r="I16" s="55"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="46">
+      <c r="I16" s="52"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="43">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="53">
+      <c r="B17" s="50">
         <v>0.125</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="55">
+      <c r="C17" s="52"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="52">
         <v>0.125</v>
       </c>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="46">
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="43">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="53">
+      <c r="B18" s="50">
         <v>1.25</v>
       </c>
-      <c r="C18" s="55">
+      <c r="C18" s="52">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D18" s="55">
+      <c r="D18" s="52">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E18" s="55">
+      <c r="E18" s="52">
         <v>0.125</v>
       </c>
-      <c r="F18" s="55">
+      <c r="F18" s="52">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G18" s="55">
+      <c r="G18" s="52">
         <v>0.1875</v>
       </c>
-      <c r="H18" s="55">
+      <c r="H18" s="52">
         <v>0.10416666666666667</v>
       </c>
-      <c r="I18" s="55">
+      <c r="I18" s="52">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J18" s="55">
+      <c r="J18" s="52">
         <v>0.16666666666666666</v>
       </c>
-      <c r="K18" s="55">
+      <c r="K18" s="52">
         <v>0.16666666666666666</v>
       </c>
-      <c r="L18" s="55">
+      <c r="L18" s="52">
         <v>0.16666666666666666</v>
       </c>
-      <c r="M18" s="55">
+      <c r="M18" s="52">
         <v>0.16666666666666666</v>
       </c>
-      <c r="N18" s="46">
+      <c r="N18" s="43">
         <f>SUM(C18:M18)</f>
         <v>1.25</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="53">
+      <c r="B19" s="50">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="55">
+      <c r="C19" s="52"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="52">
         <v>0.16666666666666666</v>
       </c>
-      <c r="J19" s="46">
+      <c r="J19" s="43">
         <v>0.16666666666666666</v>
       </c>
-      <c r="K19" s="46">
+      <c r="K19" s="43">
         <v>0.16666666666666666</v>
       </c>
-      <c r="L19" s="55">
+      <c r="L19" s="52">
         <v>0.16666666666666666</v>
       </c>
-      <c r="M19" s="56">
+      <c r="M19" s="53">
         <v>0.16666666666666666</v>
       </c>
-      <c r="N19" s="46">
+      <c r="N19" s="43">
         <f>SUM(C19:M19)</f>
         <v>0.83333333333333326</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="53">
+      <c r="B20" s="50">
         <v>0.11458333333333333</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D20" s="55">
+      <c r="D20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E20" s="55">
+      <c r="E20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="F20" s="55">
+      <c r="F20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="G20" s="55">
+      <c r="G20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="H20" s="55">
+      <c r="H20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="I20" s="55">
+      <c r="I20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="J20" s="55">
+      <c r="J20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="K20" s="55">
+      <c r="K20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="L20" s="55">
+      <c r="L20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="M20" s="55">
+      <c r="M20" s="52">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="N20" s="46">
+      <c r="N20" s="43">
         <f>SUM(C20:M20)</f>
         <v>0.11458333333333334</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="46">
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="43">
         <f>SUM(C21:M21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="46">
+      <c r="A22" s="55"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="46">
+      <c r="A23" s="49"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="46">
+      <c r="A24" s="49"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="43">
         <f>SUM(C24:M24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="46">
+      <c r="A25" s="49"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="43">
         <f>SUM(C25:M25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="46">
+      <c r="A26" s="49"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="43">
         <f>SUM(C26:M26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="46">
+      <c r="A27" s="49"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="60"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="63"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="46">
+      <c r="A28" s="57"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="61"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
-      <c r="B29" s="46">
+      <c r="A29" s="63"/>
+      <c r="B29" s="43">
         <f>SUM(B2:B28)</f>
         <v>3.65625</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29" s="43">
         <f t="shared" ref="C29:M29" si="1">SUM(C2:C28)</f>
-        <v>0.36458333333333337</v>
-      </c>
-      <c r="D29" s="46">
+        <v>0.34375</v>
+      </c>
+      <c r="D29" s="43">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="E29" s="46">
+      <c r="E29" s="43">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="F29" s="46">
+      <c r="F29" s="43">
         <f t="shared" si="1"/>
         <v>0.28125000000000006</v>
       </c>
-      <c r="G29" s="46">
+      <c r="G29" s="43">
         <f>SUM(G2:G28)</f>
         <v>0.30208333333333337</v>
       </c>
-      <c r="H29" s="46">
+      <c r="H29" s="43">
         <f t="shared" si="1"/>
         <v>0.34375000000000006</v>
       </c>
-      <c r="I29" s="46">
+      <c r="I29" s="43">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="J29" s="46">
+      <c r="J29" s="43">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="K29" s="46">
+      <c r="K29" s="43">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="L29" s="46">
+      <c r="L29" s="43">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="M29" s="46">
+      <c r="M29" s="43">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="N29" s="54"/>
+      <c r="N29" s="51"/>
     </row>
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="46">
+      <c r="A30" s="63"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="43">
         <f>SUM(C29:M29)</f>
-        <v>3.697916666666667</v>
-      </c>
-      <c r="N30" s="46">
+        <v>3.6770833333333335</v>
+      </c>
+      <c r="N30" s="43">
         <f>SUM(N2:N28)</f>
-        <v>3.6979166666666665</v>
+        <v>3.6770833333333335</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3000,127 +2971,127 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F24:F26 H24:I26 C22:C28 G22:G28 I22:I28 E22:E28 L22:L28 D18:M18 G3:G11 E3:E6 G17:G20 I3:I20 L3:L20 C4 C6:C20 D5 E8:E20 H15:H16">
-    <cfRule type="cellIs" dxfId="50" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="7" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C4:M4 C22:M26 C28:M28 C27 E27:M27 E3:M3 C3 C17:M20 C6:M6 D5:M5 C8:M11 C7 F7:M7 C12:F12 C13:E14 C15:F16 H15:M16 G14:M14 H13:M13 F13">
-    <cfRule type="cellIs" dxfId="49" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="48" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="47" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:K27 F27 H27 M27">
-    <cfRule type="cellIs" dxfId="46" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="11" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D26 G24:G26 J24:K26">
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="12" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C28:M28 C27 E27:M27 C4:M4 C17:M26 C6:M6 D5:M5 C8:M11 G7:M7 H12:M14 I15:M16">
-    <cfRule type="cellIs" dxfId="44" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C28:M28 C27 E27:M27 E3:M3 C3 C4:M4 C17:M26 C6:M6 D5:M5 C8:M11 C7 F7:M7 C12:F12 C13:E14 C15:F16 H12:M16 G14 F13">
-    <cfRule type="cellIs" dxfId="43" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C28:M28 C27 E27:M27 E3:M3 C3 C4:M4 C17:M26 C6:M6 D5:M5 C8:M11 C7 F7:M7 C12:F12 C13:E14 C15:F16 H12:M16 G14 F13">
-    <cfRule type="cellIs" dxfId="42" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:N28">
-    <cfRule type="cellIs" dxfId="41" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="16" operator="greaterThan">
       <formula>$B20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:N28">
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="17" operator="equal">
       <formula>$B20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="39" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="18" operator="greaterThan">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="38" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="19" operator="equal">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="37" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="20" operator="greaterThan">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="36" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="21" operator="equal">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N18">
-    <cfRule type="cellIs" dxfId="35" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="25" operator="greaterThan">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N18">
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="27" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="cellIs" dxfId="33" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3131,10 +3102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3202,13 +3173,15 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="6">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C2" s="7"/>
+      <c r="A2" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="36">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.125</v>
+      </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
@@ -3220,18 +3193,20 @@
       <c r="L2" s="8"/>
       <c r="M2" s="9"/>
       <c r="N2" s="10">
-        <f t="shared" ref="N2:N28" si="0">SUM(C2:M2)</f>
-        <v>0</v>
+        <f t="shared" ref="N2:N27" si="0">SUM(C2:M2)</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="11">
+      <c r="A3" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="45">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C3" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C3" s="12"/>
       <c r="D3" s="10"/>
       <c r="E3" s="12"/>
       <c r="F3" s="10"/>
@@ -3244,17 +3219,19 @@
       <c r="M3" s="13"/>
       <c r="N3" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="38">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C4" s="12"/>
+      <c r="A4" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="50">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="D4" s="10"/>
       <c r="E4" s="12"/>
       <c r="F4" s="10"/>
@@ -3267,14 +3244,14 @@
       <c r="M4" s="13"/>
       <c r="N4" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="50">
         <v>6.25E-2</v>
       </c>
       <c r="C5" s="12"/>
@@ -3294,10 +3271,10 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="50">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C6" s="12"/>
@@ -3317,22 +3294,22 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="50">
         <v>0.10416666666666667</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="12"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="12"/>
+      <c r="I7" s="14"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="12"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="13"/>
       <c r="N7" s="10">
         <f t="shared" si="0"/>
@@ -3340,15 +3317,15 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="50">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="10"/>
       <c r="G8" s="14"/>
       <c r="H8" s="10"/>
@@ -3363,13 +3340,13 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="50">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="10"/>
       <c r="E9" s="12"/>
       <c r="F9" s="10"/>
@@ -3386,10 +3363,10 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="50">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C10" s="14"/>
@@ -3409,15 +3386,15 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="50">
         <v>0.10416666666666667</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="10"/>
       <c r="G11" s="14"/>
       <c r="H11" s="10"/>
@@ -3432,15 +3409,15 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="50">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="10"/>
       <c r="G12" s="14"/>
       <c r="H12" s="10"/>
@@ -3455,17 +3432,17 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="50">
         <v>0.10416666666666667</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="10"/>
       <c r="E13" s="12"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="14"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="10"/>
       <c r="I13" s="14"/>
       <c r="J13" s="10"/>
@@ -3478,17 +3455,17 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="50">
         <v>0.125</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="12"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="16"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="10"/>
       <c r="I14" s="14"/>
       <c r="J14" s="10"/>
@@ -3501,22 +3478,22 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="50">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="14"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="10"/>
       <c r="G15" s="12"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="14"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="14"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="13"/>
       <c r="N15" s="10">
         <f t="shared" si="0"/>
@@ -3524,10 +3501,10 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="50">
         <v>0.125</v>
       </c>
       <c r="C16" s="12"/>
@@ -3547,10 +3524,10 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="50">
         <v>1.25</v>
       </c>
       <c r="C17" s="12"/>
@@ -3570,11 +3547,11 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="11">
-        <v>0.83333333333333337</v>
+      <c r="B18" s="50">
+        <v>0.79166666666666663</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="10"/>
@@ -3593,9 +3570,15 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
+      <c r="A19" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="50">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="C19" s="12">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D19" s="10"/>
       <c r="E19" s="12"/>
       <c r="F19" s="10"/>
@@ -3608,7 +3591,7 @@
       <c r="M19" s="13"/>
       <c r="N19" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3631,8 +3614,8 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="12"/>
       <c r="D21" s="10"/>
       <c r="E21" s="12"/>
@@ -3650,18 +3633,18 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="13"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="12"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="12"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="12"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="12"/>
+      <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="12"/>
+      <c r="L22" s="10"/>
       <c r="M22" s="13"/>
       <c r="N22" s="10">
         <f t="shared" si="0"/>
@@ -3672,15 +3655,15 @@
       <c r="A23" s="15"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
       <c r="M23" s="13"/>
       <c r="N23" s="10">
         <f t="shared" si="0"/>
@@ -3729,7 +3712,6 @@
       <c r="A26" s="15"/>
       <c r="B26" s="11"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -3738,109 +3720,92 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
-      <c r="M26" s="13"/>
+      <c r="M26" s="18"/>
       <c r="N26" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="18"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="24"/>
       <c r="N27" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="10">
-        <f t="shared" ref="B29:M29" si="1">SUM(B2:B28)</f>
-        <v>3.3750000000000004</v>
-      </c>
-      <c r="C29" s="10">
+      <c r="B28" s="10">
+        <f t="shared" ref="B28:M28" si="1">SUM(B2:B27)</f>
+        <v>3.6145833333333335</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="1"/>
+        <v>0.28125</v>
+      </c>
+      <c r="D28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D29" s="10">
+      <c r="E28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E29" s="10">
+      <c r="F28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F29" s="10">
+      <c r="G28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G29" s="10">
+      <c r="H28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H29" s="10">
+      <c r="I28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I29" s="10">
+      <c r="J28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J29" s="10">
+      <c r="K28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K29" s="10">
+      <c r="L28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L29" s="10">
+      <c r="M28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M29" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M30" s="10">
-        <f>SUM(C29:M29)</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="10">
-        <f>SUM(N2:N28)</f>
-        <v>0</v>
-      </c>
-    </row>
+        <f>SUM(C28:M28)</f>
+        <v>0.28125</v>
+      </c>
+      <c r="N29" s="10">
+        <f>SUM(N2:N27)</f>
+        <v>0.28125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4810,91 +4775,80 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:M2 F24:F26 H24:I26 C3:C20 E3:E20 G3:G20 I3:I20 L3:L20 C22:C28 G22:G28 I22:I23 I27:I28 E22:E28 L22:L28">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 F23:F25 H23:I25 C21:C27 G21:G27 I21:I22 I26:I27 E21:E27 L21:L27 C3:C19 E3:E19 G3:G19 I3:I19 L3:L19">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M2 C4:M11 C13:M20 C22:M26 C28:M28 C27 E27:M27">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M25">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="L20 I20 G20 E20 C20">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="C20:M20">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J27:K27 F27 H27 M27">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="J26:K26 F26 H26 M26">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D26 G24:G26 J24:K26">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="D23:D25 G23:G25 J23:K25">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M26 C28:M28 C27 E27:M27">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27 C26 E26:M26">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M26 C28:M28 C27 E27:M27">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M25">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M26 C28:M28 C27 E27:M27">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M25">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="greaterThan">
+  <conditionalFormatting sqref="N2:N27">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+  <conditionalFormatting sqref="N2:N27">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="greaterThan">
+  <conditionalFormatting sqref="B28">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+  <conditionalFormatting sqref="B28">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+  <conditionalFormatting sqref="C28:M28">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="greaterThan">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+  <conditionalFormatting sqref="C28:M28">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>0.3333333333</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N28">
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="greaterThan">
-      <formula>$B3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N28">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
-      <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
avancement de la doc
</commit_message>
<xml_diff>
--- a/annexes/Planification.xlsx
+++ b/annexes/Planification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -151,9 +151,6 @@
     <t>vérification de l'email</t>
   </si>
   <si>
-    <t>envoie du mail avec la clé de vérification</t>
-  </si>
-  <si>
     <t>ajout dans les logs après 3 echecs</t>
   </si>
   <si>
@@ -200,6 +197,42 @@
   </si>
   <si>
     <t>Journal de bord</t>
+  </si>
+  <si>
+    <t>Vérification de l'email</t>
+  </si>
+  <si>
+    <t>Formulaire d'identification (email - mot de passe) / login</t>
+  </si>
+  <si>
+    <t>Ajout dans les logs après 3 echecs</t>
+  </si>
+  <si>
+    <t>Formulaire récupération du mot de passe / envoie du mail</t>
+  </si>
+  <si>
+    <t>Modification du mot de passe après la redirection</t>
+  </si>
+  <si>
+    <t>Faire la page du profil</t>
+  </si>
+  <si>
+    <t>Modification du profil</t>
+  </si>
+  <si>
+    <t>Consultation des logs pour l'admin</t>
+  </si>
+  <si>
+    <t>Afficher les utilisateurs avec filtre de recherche par nom, prénom, email(admin)</t>
+  </si>
+  <si>
+    <t>Modification des users pour l'admin / mail pour informer</t>
+  </si>
+  <si>
+    <t>Suppression d'un utilisateurs (pas possible si il a des commandes et actifs il y a moin d'un an)</t>
+  </si>
+  <si>
+    <t>CRUD sur la table catégorie</t>
   </si>
 </sst>
 </file>
@@ -584,7 +617,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -780,6 +869,22 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFD6E3BC"/>
+          <bgColor rgb="FFD6E3BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBD4B4"/>
+          <bgColor rgb="FFFBD4B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
         </patternFill>
@@ -934,22 +1039,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1188,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1260,7 +1349,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="36">
         <v>0.16666666666666666</v>
@@ -1279,7 +1368,7 @@
       <c r="L2" s="47"/>
       <c r="M2" s="48"/>
       <c r="N2" s="43">
-        <f t="shared" ref="N2:N28" si="0">SUM(C2:M2)</f>
+        <f t="shared" ref="N2:N26" si="0">SUM(C2:M2)</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -1288,7 +1377,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="45">
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C3" s="43">
         <v>4.1666666666666664E-2</v>
@@ -1310,7 +1399,7 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B4" s="50">
         <v>8.3333333333333329E-2</v>
@@ -1335,13 +1424,14 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B5" s="50">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D5" s="52">
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="43">
+        <v>6.25E-2</v>
       </c>
       <c r="E5" s="52"/>
       <c r="F5" s="43"/>
@@ -1353,23 +1443,21 @@
       <c r="L5" s="52"/>
       <c r="M5" s="53"/>
       <c r="N5" s="43">
-        <f>SUM(D5:M5)</f>
-        <v>4.1666666666666664E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B6" s="50">
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C6" s="52"/>
-      <c r="D6" s="43">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="43"/>
+      <c r="F6" s="43">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G6" s="52"/>
       <c r="H6" s="43"/>
       <c r="I6" s="52"/>
@@ -1379,44 +1467,46 @@
       <c r="M6" s="53"/>
       <c r="N6" s="43">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B7" s="50">
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C7" s="52"/>
-      <c r="F7" s="43">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G7" s="52"/>
+      <c r="D7" s="43">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E7" s="54"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="43"/>
-      <c r="I7" s="52"/>
+      <c r="I7" s="54"/>
       <c r="J7" s="43"/>
       <c r="K7" s="43"/>
-      <c r="L7" s="52"/>
+      <c r="L7" s="54"/>
       <c r="M7" s="53"/>
       <c r="N7" s="43">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B8" s="50">
-        <v>0.10416666666666667</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C8" s="52"/>
       <c r="D8" s="43">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="E8" s="54"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E8" s="52"/>
       <c r="F8" s="43"/>
       <c r="G8" s="54"/>
       <c r="H8" s="43"/>
@@ -1427,21 +1517,21 @@
       <c r="M8" s="53"/>
       <c r="N8" s="43">
         <f t="shared" si="0"/>
-        <v>0.10416666666666667</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B9" s="50">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="43">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E9" s="52"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C9" s="54"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="52">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="F9" s="43"/>
       <c r="G9" s="54"/>
       <c r="H9" s="43"/>
@@ -1452,23 +1542,22 @@
       <c r="M9" s="53"/>
       <c r="N9" s="43">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B10" s="50">
-        <v>0.16666666666666666</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C10" s="54"/>
       <c r="D10" s="43"/>
-      <c r="E10" s="52">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="43">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="H10" s="43"/>
       <c r="I10" s="54"/>
       <c r="J10" s="43"/>
@@ -1477,23 +1566,22 @@
       <c r="M10" s="53"/>
       <c r="N10" s="43">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B11" s="50">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C11" s="54"/>
       <c r="D11" s="43"/>
-      <c r="E11" s="52">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="54"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="43">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="H11" s="43"/>
       <c r="I11" s="54"/>
       <c r="J11" s="43"/>
@@ -1502,20 +1590,20 @@
       <c r="M11" s="53"/>
       <c r="N11" s="43">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B12" s="50">
         <v>0.10416666666666667</v>
       </c>
       <c r="C12" s="54"/>
       <c r="D12" s="43"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="43">
+      <c r="E12" s="52"/>
+      <c r="G12" s="43">
         <v>0.10416666666666667</v>
       </c>
       <c r="H12" s="43"/>
@@ -1531,18 +1619,18 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B13" s="50">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="C13" s="54"/>
       <c r="D13" s="43"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="43">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H13" s="43"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="43"/>
+      <c r="H13" s="52">
+        <v>0.125</v>
+      </c>
       <c r="I13" s="54"/>
       <c r="J13" s="43"/>
       <c r="K13" s="43"/>
@@ -1550,27 +1638,27 @@
       <c r="M13" s="53"/>
       <c r="N13" s="43">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B14" s="50">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C14" s="54"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="43"/>
       <c r="E14" s="52"/>
-      <c r="G14" s="43">
+      <c r="F14" s="43"/>
+      <c r="H14" s="52">
         <v>0.10416666666666667</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="54"/>
+      <c r="I14" s="52"/>
       <c r="J14" s="43"/>
       <c r="K14" s="43"/>
-      <c r="L14" s="54"/>
+      <c r="L14" s="52"/>
       <c r="M14" s="53"/>
       <c r="N14" s="43">
         <f t="shared" si="0"/>
@@ -1579,58 +1667,78 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B15" s="50">
-        <v>0.125</v>
-      </c>
-      <c r="C15" s="54"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C15" s="52"/>
       <c r="D15" s="43"/>
-      <c r="E15" s="54"/>
+      <c r="E15" s="52"/>
       <c r="F15" s="43"/>
-      <c r="H15" s="52">
-        <v>0.125</v>
-      </c>
-      <c r="I15" s="54"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="52">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="J15" s="43"/>
       <c r="K15" s="43"/>
-      <c r="L15" s="54"/>
+      <c r="L15" s="52"/>
       <c r="M15" s="53"/>
       <c r="N15" s="43">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B16" s="50">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="43"/>
+        <v>1.25</v>
+      </c>
+      <c r="C16" s="52">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D16" s="52">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E16" s="52">
+        <v>0.125</v>
+      </c>
+      <c r="F16" s="52">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G16" s="52">
+        <v>0.1875</v>
+      </c>
       <c r="H16" s="52">
         <v>0.10416666666666667</v>
       </c>
       <c r="I16" s="52"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="53"/>
+      <c r="J16" s="52">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K16" s="52">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="L16" s="52">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M16" s="52">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="N16" s="43">
-        <f t="shared" si="0"/>
-        <v>0.10416666666666667</v>
+        <f>SUM(C16:M16)</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="50">
-        <v>0.125</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C17" s="52"/>
       <c r="D17" s="43"/>
@@ -1639,138 +1747,106 @@
       <c r="G17" s="52"/>
       <c r="H17" s="43"/>
       <c r="I17" s="52">
-        <v>0.125</v>
-      </c>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="53"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J17" s="43">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K17" s="43">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="L17" s="52">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M17" s="53">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="N17" s="43">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
+        <f>SUM(C17:M17)</f>
+        <v>0.83333333333333326</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" s="50">
-        <v>1.25</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="C18" s="52">
-        <v>4.1666666666666664E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="D18" s="52">
-        <v>4.1666666666666664E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="E18" s="52">
-        <v>0.125</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="F18" s="52">
-        <v>4.1666666666666664E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="G18" s="52">
-        <v>0.1875</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="H18" s="52">
-        <v>0.10416666666666667</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="I18" s="52">
-        <v>4.1666666666666664E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="J18" s="52">
-        <v>0.16666666666666666</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="K18" s="52">
-        <v>0.16666666666666666</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="L18" s="52">
-        <v>0.16666666666666666</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="M18" s="52">
-        <v>0.16666666666666666</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="N18" s="43">
         <f>SUM(C18:M18)</f>
-        <v>1.25</v>
+        <v>0.1423611111111111</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="50">
-        <v>0.79166666666666663</v>
-      </c>
+      <c r="A19" s="49"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="52"/>
       <c r="D19" s="43"/>
       <c r="E19" s="52"/>
       <c r="F19" s="43"/>
       <c r="G19" s="52"/>
       <c r="H19" s="43"/>
-      <c r="I19" s="52">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="J19" s="43">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K19" s="43">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="L19" s="52">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="M19" s="53">
-        <v>0.16666666666666666</v>
-      </c>
+      <c r="I19" s="52"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="53"/>
       <c r="N19" s="43">
         <f>SUM(C19:M19)</f>
-        <v>0.83333333333333326</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="50">
-        <v>0.11458333333333333</v>
-      </c>
-      <c r="C20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="D20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="F20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="G20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="H20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="I20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="J20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="K20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="L20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="M20" s="52">
-        <v>1.0416666666666666E-2</v>
-      </c>
+      <c r="A20" s="55"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="53"/>
       <c r="N20" s="43">
-        <f>SUM(C20:M20)</f>
-        <v>0.11458333333333334</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1778,36 +1854,36 @@
       <c r="B21" s="50"/>
       <c r="C21" s="52"/>
       <c r="D21" s="43"/>
-      <c r="E21" s="52"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="43"/>
-      <c r="G21" s="52"/>
+      <c r="G21" s="43"/>
       <c r="H21" s="43"/>
-      <c r="I21" s="52"/>
+      <c r="I21" s="43"/>
       <c r="J21" s="43"/>
       <c r="K21" s="43"/>
-      <c r="L21" s="52"/>
+      <c r="L21" s="43"/>
       <c r="M21" s="53"/>
       <c r="N21" s="43">
-        <f>SUM(C21:M21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="53"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="52"/>
-      <c r="D22" s="43"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="52"/>
-      <c r="F22" s="43"/>
+      <c r="F22" s="52"/>
       <c r="G22" s="52"/>
-      <c r="H22" s="43"/>
+      <c r="H22" s="52"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
       <c r="L22" s="52"/>
       <c r="M22" s="53"/>
       <c r="N22" s="43">
-        <f t="shared" si="0"/>
+        <f>SUM(C22:M22)</f>
         <v>0</v>
       </c>
     </row>
@@ -1815,18 +1891,18 @@
       <c r="A23" s="49"/>
       <c r="B23" s="50"/>
       <c r="C23" s="52"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
       <c r="M23" s="53"/>
       <c r="N23" s="43">
-        <f t="shared" si="0"/>
+        <f>SUM(C23:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -1853,7 +1929,7 @@
       <c r="A25" s="49"/>
       <c r="B25" s="50"/>
       <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
+      <c r="D25" s="51"/>
       <c r="E25" s="52"/>
       <c r="F25" s="52"/>
       <c r="G25" s="52"/>
@@ -1862,143 +1938,107 @@
       <c r="J25" s="52"/>
       <c r="K25" s="52"/>
       <c r="L25" s="52"/>
-      <c r="M25" s="53"/>
+      <c r="M25" s="56"/>
       <c r="N25" s="43">
-        <f>SUM(C25:M25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="43">
-        <f>SUM(C26:M26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="57"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="62"/>
-      <c r="N28" s="43">
+    <row r="26" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="57"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="63"/>
-      <c r="B29" s="43">
-        <f>SUM(B2:B28)</f>
-        <v>3.65625</v>
-      </c>
-      <c r="C29" s="43">
-        <f t="shared" ref="C29:M29" si="1">SUM(C2:C28)</f>
+    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="63"/>
+      <c r="B27" s="43">
+        <f>SUM(B2:B26)</f>
+        <v>3.6631944444444446</v>
+      </c>
+      <c r="C27" s="43">
+        <f>SUM(C2:C26)</f>
         <v>0.34375</v>
       </c>
-      <c r="D29" s="43">
-        <f t="shared" si="1"/>
+      <c r="D27" s="43">
+        <f>SUM(D2:D26)</f>
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="E27" s="43">
+        <f>SUM(E2:E26)</f>
+        <v>0.30902777777777773</v>
+      </c>
+      <c r="F27" s="43">
+        <f>SUM(F2:F26)</f>
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="G27" s="43">
+        <f>SUM(G2:G26)</f>
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="H27" s="43">
+        <f>SUM(H2:H26)</f>
+        <v>0.34375000000000006</v>
+      </c>
+      <c r="I27" s="43">
+        <f>SUM(I2:I26)</f>
         <v>0.34375</v>
       </c>
-      <c r="E29" s="43">
-        <f t="shared" si="1"/>
+      <c r="J27" s="43">
+        <f>SUM(J2:J26)</f>
         <v>0.34375</v>
       </c>
-      <c r="F29" s="43">
-        <f t="shared" si="1"/>
-        <v>0.28125000000000006</v>
-      </c>
-      <c r="G29" s="43">
-        <f>SUM(G2:G28)</f>
-        <v>0.30208333333333337</v>
-      </c>
-      <c r="H29" s="43">
-        <f t="shared" si="1"/>
-        <v>0.34375000000000006</v>
-      </c>
-      <c r="I29" s="43">
-        <f t="shared" si="1"/>
+      <c r="K27" s="43">
+        <f>SUM(K2:K26)</f>
         <v>0.34375</v>
       </c>
-      <c r="J29" s="43">
-        <f t="shared" si="1"/>
+      <c r="L27" s="43">
+        <f>SUM(L2:L26)</f>
         <v>0.34375</v>
       </c>
-      <c r="K29" s="43">
-        <f t="shared" si="1"/>
+      <c r="M27" s="43">
+        <f>SUM(M2:M26)</f>
         <v>0.34375</v>
       </c>
-      <c r="L29" s="43">
-        <f t="shared" si="1"/>
-        <v>0.34375</v>
-      </c>
-      <c r="M29" s="43">
-        <f t="shared" si="1"/>
-        <v>0.34375</v>
-      </c>
-      <c r="N29" s="51"/>
-    </row>
-    <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="63"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="43">
-        <f>SUM(C29:M29)</f>
-        <v>3.6770833333333335</v>
-      </c>
-      <c r="N30" s="43">
-        <f>SUM(N2:N28)</f>
-        <v>3.6770833333333335</v>
-      </c>
-    </row>
+      <c r="N27" s="51"/>
+    </row>
+    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="63"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="43">
+        <f>SUM(C27:M27)</f>
+        <v>3.6631944444444446</v>
+      </c>
+      <c r="N28" s="43">
+        <f>SUM(N2:N26)</f>
+        <v>3.6631944444444442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2967,131 +3007,149 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:M2 F24:F26 H24:I26 C22:C28 G22:G28 I22:I28 E22:E28 L22:L28 D18:M18 G3:G11 E3:E6 G17:G20 I3:I20 L3:L20 C4 C6:C20 D5 E8:E20 H15:H16">
-    <cfRule type="cellIs" dxfId="48" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 F22:F24 H22:I24 C20:C26 G20:G26 I20:I26 E20:E26 L20:L26 D16:M16 H13:H14 G3:G9 E3:E5 C4:C18 I3:I18 L3:L18 E7:E18 G15:G18">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M2 C4:M4 C22:M26 C28:M28 C27 E27:M27 E3:M3 C3 C17:M20 C6:M6 D5:M5 C8:M11 C7 F7:M7 C12:F12 C13:E14 C15:F16 H15:M16 G14:M14 H13:M13 F13">
-    <cfRule type="cellIs" dxfId="47" priority="8" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 C20:M24 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H13:M14 G12:M12 H11:M11 F11 C15:M18">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="46" priority="9" operator="greaterThan">
+  <conditionalFormatting sqref="L19 I19 G19 E19 C19">
+    <cfRule type="cellIs" dxfId="55" priority="11" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="45" priority="10" operator="greaterThan">
+  <conditionalFormatting sqref="C19:M19">
+    <cfRule type="cellIs" dxfId="54" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J27:K27 F27 H27 M27">
-    <cfRule type="cellIs" dxfId="44" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="J25:K25 F25 H25 M25">
+    <cfRule type="cellIs" dxfId="53" priority="13" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D26 G24:G26 J24:K26">
-    <cfRule type="cellIs" dxfId="43" priority="12" operator="greaterThan">
+  <conditionalFormatting sqref="D22:D24 G22:G24 J22:K24">
+    <cfRule type="cellIs" dxfId="52" priority="14" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M2 C28:M28 C27 E27:M27 C4:M4 C17:M26 C6:M6 D5:M5 C8:M11 G7:M7 H12:M14 I15:M16">
-    <cfRule type="cellIs" dxfId="42" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 C4:M5 C7:M9 G6:M6 H10:M12 I13:M14 C15:M24">
+    <cfRule type="cellIs" dxfId="51" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M2 C28:M28 C27 E27:M27 E3:M3 C3 C4:M4 C17:M26 C6:M6 D5:M5 C8:M11 C7 F7:M7 C12:F12 C13:E14 C15:F16 H12:M16 G14 F13">
-    <cfRule type="cellIs" dxfId="41" priority="14" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H10:M14 G12 F11 C15:M24">
+    <cfRule type="cellIs" dxfId="50" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M2 C28:M28 C27 E27:M27 E3:M3 C3 C4:M4 C17:M26 C6:M6 D5:M5 C8:M11 C7 F7:M7 C12:F12 C13:E14 C15:F16 H12:M16 G14 F13">
-    <cfRule type="cellIs" dxfId="40" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H10:M14 G12 F11 C15:M24">
+    <cfRule type="cellIs" dxfId="49" priority="17" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N20:N28">
-    <cfRule type="cellIs" dxfId="39" priority="16" operator="greaterThan">
-      <formula>$B20</formula>
+  <conditionalFormatting sqref="N18:N26">
+    <cfRule type="cellIs" dxfId="48" priority="18" operator="greaterThan">
+      <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N20:N28">
-    <cfRule type="cellIs" dxfId="38" priority="17" operator="equal">
-      <formula>$B20</formula>
+  <conditionalFormatting sqref="N18:N26">
+    <cfRule type="cellIs" dxfId="47" priority="19" operator="equal">
+      <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="37" priority="18" operator="greaterThan">
+  <conditionalFormatting sqref="B27">
+    <cfRule type="cellIs" dxfId="46" priority="20" operator="greaterThan">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="36" priority="19" operator="equal">
+  <conditionalFormatting sqref="B27">
+    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="35" priority="20" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27">
+    <cfRule type="cellIs" dxfId="44" priority="22" operator="greaterThan">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="34" priority="21" operator="equal">
+  <conditionalFormatting sqref="C27:M27">
+    <cfRule type="cellIs" dxfId="43" priority="23" operator="equal">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N18">
-    <cfRule type="cellIs" dxfId="33" priority="25" operator="greaterThan">
+  <conditionalFormatting sqref="N2:N3 N5:N8 N10:N16">
+    <cfRule type="cellIs" dxfId="42" priority="27" operator="greaterThan">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N18">
-    <cfRule type="cellIs" dxfId="32" priority="27" operator="equal">
+  <conditionalFormatting sqref="N2:N3 N5:N8 N10:N16">
+    <cfRule type="cellIs" dxfId="41" priority="29" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N19">
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="greaterThan">
+  <conditionalFormatting sqref="N17">
+    <cfRule type="cellIs" dxfId="40" priority="32" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N19">
-    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
+  <conditionalFormatting sqref="N17">
+    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="M18">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="D18">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="H18">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J20">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="J18">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="K18">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4 N9">
+    <cfRule type="cellIs" dxfId="32" priority="47" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4 N9">
+    <cfRule type="cellIs" dxfId="31" priority="50" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3104,8 +3162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3174,7 +3232,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="36">
         <v>0.16666666666666666</v>
@@ -3249,7 +3307,7 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="50">
         <v>6.25E-2</v>
@@ -3272,7 +3330,7 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="50">
         <v>4.1666666666666664E-2</v>
@@ -3295,7 +3353,7 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="50">
         <v>0.10416666666666667</v>
@@ -3318,7 +3376,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="50">
         <v>8.3333333333333329E-2</v>
@@ -3341,7 +3399,7 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="50">
         <v>0.16666666666666666</v>
@@ -3364,7 +3422,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="50">
         <v>4.1666666666666664E-2</v>
@@ -3387,7 +3445,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="50">
         <v>0.10416666666666667</v>
@@ -3410,7 +3468,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="50">
         <v>8.3333333333333329E-2</v>
@@ -3433,7 +3491,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="50">
         <v>0.10416666666666667</v>
@@ -3456,7 +3514,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="50">
         <v>0.125</v>
@@ -3479,7 +3537,7 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="50">
         <v>0.10416666666666667</v>
@@ -3502,7 +3560,7 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="50">
         <v>0.125</v>
@@ -3525,7 +3583,7 @@
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="50">
         <v>1.25</v>
@@ -3548,7 +3606,7 @@
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="50">
         <v>0.79166666666666663</v>
@@ -3571,7 +3629,7 @@
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="50">
         <v>0.11458333333333333</v>
@@ -4777,77 +4835,77 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F23:F25 H23:I25 C21:C27 G21:G27 I21:I22 I26:I27 E21:E27 L21:L27 C3:C19 E3:E19 G3:G19 I3:I19 L3:L19">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M25">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20 I20 G20 E20 C20">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:K26 F26 H26 M26">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25 G23:G25 J23:K25">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27 C26 E26:M26">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M25">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M25">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N27">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N27">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="greaterThan">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:M28">
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="greaterThan">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:M28">
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6571,47 +6629,47 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:L2 F24 H24:I24 C3:C20 E3:E20 G3:G20 I3:I20 K3:K20 C22:C26 G22:G26 I22:I23 I25:I26 E22:E26 K22:K26">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L2 C4:L11 C13:L20 C22:L26">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:L21">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 F25 H25 J25 L25">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24 G24 J24">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L26">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L26">
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L26">
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ajout du systme de log
</commit_message>
<xml_diff>
--- a/annexes/Planification.xlsx
+++ b/annexes/Planification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -73,45 +73,6 @@
   </si>
   <si>
     <t>Inscription générale (formulaire simple)</t>
-  </si>
-  <si>
-    <t>vérification de l'email</t>
-  </si>
-  <si>
-    <t>ajout dans les logs après 3 echecs</t>
-  </si>
-  <si>
-    <t>formulaire d'identification (email - mot de passe) / login</t>
-  </si>
-  <si>
-    <t>formulaire récupération du mot de passe / envoie du mail</t>
-  </si>
-  <si>
-    <t>modification du mot de passe après la redirection</t>
-  </si>
-  <si>
-    <t>faire la page du profil</t>
-  </si>
-  <si>
-    <t>modification du profil</t>
-  </si>
-  <si>
-    <t>consultation des logs pour l'admin</t>
-  </si>
-  <si>
-    <t>afficher les utilisateurs avec filtre de recherche par nom, prénom, email(admin)</t>
-  </si>
-  <si>
-    <t>modification des users pour l'admin / mail pour informer</t>
-  </si>
-  <si>
-    <t>suppression d'un utilisateurs (pas possible si il a des commandes et actifs il y a moin d'un an)</t>
-  </si>
-  <si>
-    <t>crud sur la table catégorie</t>
-  </si>
-  <si>
-    <t>documentation</t>
   </si>
   <si>
     <t>Tests</t>
@@ -1086,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1156,7 +1117,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B2" s="25">
         <v>0.16666666666666666</v>
@@ -1206,7 +1167,7 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B4" s="39">
         <v>8.3333333333333329E-2</v>
@@ -1231,7 +1192,7 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B5" s="39">
         <v>6.25E-2</v>
@@ -1256,7 +1217,7 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B6" s="39">
         <v>4.1666666666666664E-2</v>
@@ -1279,7 +1240,7 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B7" s="39">
         <v>0.10416666666666667</v>
@@ -1304,7 +1265,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B8" s="39">
         <v>8.3333333333333329E-2</v>
@@ -1329,7 +1290,7 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B9" s="39">
         <v>0.16666666666666666</v>
@@ -1354,7 +1315,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B10" s="39">
         <v>0.10416666666666667</v>
@@ -1378,7 +1339,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B11" s="39">
         <v>8.3333333333333329E-2</v>
@@ -1402,7 +1363,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B12" s="39">
         <v>0.10416666666666667</v>
@@ -1426,7 +1387,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B13" s="39">
         <v>0.125</v>
@@ -1450,7 +1411,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B14" s="39">
         <v>0.10416666666666667</v>
@@ -1474,7 +1435,7 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B15" s="39">
         <v>0.16666666666666666</v>
@@ -1542,7 +1503,7 @@
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B17" s="39">
         <v>0.83333333333333337</v>
@@ -1575,7 +1536,7 @@
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B18" s="39">
         <v>0.1423611111111111</v>
@@ -2969,8 +2930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3039,7 +3000,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B2" s="25">
         <v>0.16666666666666666</v>
@@ -3067,7 +3028,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="34">
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C3" s="11">
         <v>4.1666666666666664E-2</v>
@@ -3089,7 +3050,7 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="39">
         <v>8.3333333333333329E-2</v>
@@ -3114,7 +3075,7 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="39">
         <v>6.25E-2</v>
@@ -3139,7 +3100,7 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" s="39">
         <v>4.1666666666666664E-2</v>
@@ -3147,7 +3108,9 @@
       <c r="C6" s="11"/>
       <c r="D6" s="9"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9">
+        <v>6.25E-2</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="9"/>
       <c r="I6" s="11"/>
@@ -3157,12 +3120,12 @@
       <c r="M6" s="12"/>
       <c r="N6" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B7" s="39">
         <v>0.10416666666666667</v>
@@ -3187,7 +3150,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B8" s="39">
         <v>8.3333333333333329E-2</v>
@@ -3212,7 +3175,7 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" s="39">
         <v>0.16666666666666666</v>
@@ -3237,7 +3200,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B10" s="39">
         <v>0.10416666666666667</v>
@@ -3262,7 +3225,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B11" s="39">
         <v>8.3333333333333329E-2</v>
@@ -3270,7 +3233,9 @@
       <c r="C11" s="13"/>
       <c r="D11" s="9"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="9">
+        <v>6.9444444444444434E-2</v>
+      </c>
       <c r="G11" s="13"/>
       <c r="H11" s="9"/>
       <c r="I11" s="13"/>
@@ -3280,12 +3245,12 @@
       <c r="M11" s="12"/>
       <c r="N11" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444434E-2</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B12" s="39">
         <v>0.10416666666666667</v>
@@ -3308,7 +3273,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B13" s="39">
         <v>0.125</v>
@@ -3331,7 +3296,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="39">
         <v>0.10416666666666667</v>
@@ -3354,10 +3319,10 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B15" s="39">
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="9"/>
@@ -3377,7 +3342,7 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B16" s="39">
         <v>1.25</v>
@@ -3406,10 +3371,10 @@
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B17" s="39">
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="9">
@@ -3431,10 +3396,10 @@
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B18" s="39">
-        <v>0.11458333333333333</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="C18" s="11">
         <v>1.0416666666666666E-2</v>
@@ -3612,7 +3577,7 @@
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
         <f t="shared" ref="B27:M27" si="1">SUM(B2:B26)</f>
-        <v>3.572916666666667</v>
+        <v>3.6631944444444446</v>
       </c>
       <c r="C27" s="9">
         <f t="shared" si="1"/>
@@ -3628,7 +3593,7 @@
       </c>
       <c r="F27" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.13194444444444442</v>
       </c>
       <c r="G27" s="9">
         <f t="shared" si="1"/>
@@ -3662,11 +3627,11 @@
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M28" s="9">
         <f>SUM(C27:M27)</f>
-        <v>1.0208333333333333</v>
+        <v>1.1527777777777777</v>
       </c>
       <c r="N28" s="9">
         <f>SUM(N2:N26)</f>
-        <v>1.0208333333333335</v>
+        <v>1.1527777777777777</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Ajout du filtrage et de la pagination sur l'affichage des users
</commit_message>
<xml_diff>
--- a/annexes/Planification.xlsx
+++ b/annexes/Planification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -119,6 +119,9 @@
   <si>
     <t>CRUD sur la table catégorie</t>
   </si>
+  <si>
+    <t xml:space="preserve">L'admin peut créer un utilisateur </t>
+  </si>
 </sst>
 </file>
 
@@ -127,19 +130,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -172,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -377,6 +374,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -407,10 +415,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -418,62 +422,98 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD6E3BC"/>
+          <bgColor rgb="FFD6E3BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBD4B4"/>
+          <bgColor rgb="FFFBD4B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD6E3BC"/>
+          <bgColor rgb="FFD6E3BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBD4B4"/>
+          <bgColor rgb="FFFBD4B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1047,59 +1087,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="73.125" style="22" customWidth="1"/>
     <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="13" width="10.125" customWidth="1"/>
     <col min="14" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="28" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="5"/>
@@ -1116,691 +1156,691 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="33">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="32">
+      <c r="D2" s="34"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="30">
         <f t="shared" ref="N2:N26" si="0">SUM(C2:M2)</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="30">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="32">
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="30">
         <f>SUM(C3:M3)</f>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="37">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="39">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="32">
+      <c r="D4" s="30"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="30">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>6.25E-2</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="32">
+      <c r="C5" s="39"/>
+      <c r="D5" s="30">
         <v>6.25E-2</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="32">
+      <c r="E5" s="39"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="30">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="F6" s="32">
+      <c r="C6" s="39"/>
+      <c r="F6" s="30">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="32">
+      <c r="G6" s="39"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="30">
         <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="32">
+      <c r="C7" s="39"/>
+      <c r="D7" s="30">
         <v>0.10416666666666667</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="32">
+      <c r="E7" s="41"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="30">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="32">
+      <c r="C8" s="39"/>
+      <c r="D8" s="30">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="32">
+      <c r="E8" s="39"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="30">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="41">
+      <c r="C9" s="41"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="32">
+      <c r="F9" s="30"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="30">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="32">
+      <c r="C10" s="41"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="30">
         <v>0.10416666666666667</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="32">
+      <c r="H10" s="30"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="30">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="32">
+      <c r="C11" s="41"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="30">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="32">
+      <c r="H11" s="30"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="30">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="41"/>
-      <c r="G12" s="32">
+      <c r="C12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="39"/>
+      <c r="G12" s="30">
         <v>0.10416666666666667</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="32">
+      <c r="H12" s="30"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="30">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>0.125</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="32"/>
-      <c r="H13" s="41">
+      <c r="C13" s="41"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="30"/>
+      <c r="H13" s="39">
         <v>0.125</v>
       </c>
-      <c r="I13" s="43"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="32">
+      <c r="I13" s="41"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="30">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="37">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="32"/>
-      <c r="H14" s="41">
+      <c r="C14" s="39"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="30"/>
+      <c r="H14" s="39">
         <v>0.10416666666666667</v>
       </c>
-      <c r="I14" s="41"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="32">
+      <c r="I14" s="39"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="30">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B15" s="37">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="41">
+      <c r="C15" s="39"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="32">
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="30">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="39">
+      <c r="B16" s="37">
         <v>1.25</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="39">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="39">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="39">
         <v>0.125</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="39">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="39">
         <v>0.1875</v>
       </c>
-      <c r="H16" s="41">
+      <c r="H16" s="39">
         <v>0.10416666666666667</v>
       </c>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41">
+      <c r="I16" s="39"/>
+      <c r="J16" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="K16" s="41">
+      <c r="K16" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="L16" s="41">
+      <c r="L16" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="M16" s="41">
+      <c r="M16" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="N16" s="32">
+      <c r="N16" s="30">
         <f>SUM(C16:M16)</f>
         <v>1.25</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="39">
+      <c r="B17" s="37">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="41">
+      <c r="C17" s="39"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="30">
         <v>0.16666666666666666</v>
       </c>
-      <c r="K17" s="32">
+      <c r="K17" s="30">
         <v>0.16666666666666666</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M17" s="40">
         <v>0.16666666666666666</v>
       </c>
-      <c r="N17" s="32">
+      <c r="N17" s="30">
         <f>SUM(C17:M17)</f>
         <v>0.83333333333333326</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="39">
+      <c r="B18" s="37">
         <v>0.1423611111111111</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="39">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D18" s="41">
+      <c r="D18" s="39">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="39">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="F18" s="41">
+      <c r="F18" s="39">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="39">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="H18" s="41">
+      <c r="H18" s="39">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="I18" s="41">
+      <c r="I18" s="39">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="J18" s="41">
+      <c r="J18" s="39">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="K18" s="41">
+      <c r="K18" s="39">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="L18" s="41">
+      <c r="L18" s="39">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="M18" s="41">
+      <c r="M18" s="39">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="N18" s="32">
+      <c r="N18" s="30">
         <f>SUM(C18:M18)</f>
         <v>0.1423611111111111</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="32">
+      <c r="A19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="30">
         <f>SUM(C19:M19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="32">
+      <c r="A20" s="42"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="32">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="32">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="30">
         <f>SUM(C22:M22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="32">
+      <c r="A23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="30">
         <f>SUM(C23:M23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="32">
+      <c r="A24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="30">
         <f>SUM(C24:M24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="32">
+      <c r="A25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="32">
+      <c r="A26" s="44"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="32">
+      <c r="A27" s="50"/>
+      <c r="B27" s="30">
         <f t="shared" ref="B27:M27" si="1">SUM(B2:B26)</f>
         <v>3.6631944444444446</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="30">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="30">
         <f t="shared" si="1"/>
         <v>0.30902777777777779</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="30">
         <f t="shared" si="1"/>
         <v>0.30902777777777773</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="30">
         <f t="shared" si="1"/>
         <v>0.3298611111111111</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="30">
         <f t="shared" si="1"/>
         <v>0.30902777777777779</v>
       </c>
-      <c r="H27" s="32">
+      <c r="H27" s="30">
         <f t="shared" si="1"/>
         <v>0.34375000000000006</v>
       </c>
-      <c r="I27" s="32">
+      <c r="I27" s="30">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="J27" s="32">
+      <c r="J27" s="30">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="K27" s="32">
+      <c r="K27" s="30">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="L27" s="32">
+      <c r="L27" s="30">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="M27" s="32">
+      <c r="M27" s="30">
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="N27" s="40"/>
+      <c r="N27" s="38"/>
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="32">
+      <c r="A28" s="50"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="30">
         <f>SUM(C27:M27)</f>
         <v>3.6631944444444446</v>
       </c>
-      <c r="N28" s="32">
+      <c r="N28" s="30">
         <f>SUM(N2:N26)</f>
         <v>3.6631944444444442</v>
       </c>
@@ -2777,147 +2817,147 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F22:F24 H22:I24 C20:C26 G20:G26 I20:I26 E20:E26 L20:L26 D16:M16 H13:H14 G3:G9 E3:E5 C4:C18 I3:I18 L3:L18 E7:E18 G15:G18">
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C20:M24 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H13:M14 G12:M12 H11:M11 F11 C15:M18">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19 I19 G19 E19 C19">
-    <cfRule type="cellIs" dxfId="42" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="11" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:K25 F25 H25 M25">
-    <cfRule type="cellIs" dxfId="40" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="13" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:D24 G22:G24 J22:K24">
-    <cfRule type="cellIs" dxfId="39" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="14" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 C4:M5 C7:M9 G6:M6 H10:M12 I13:M14 C15:M24">
-    <cfRule type="cellIs" dxfId="38" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H10:M14 G12 F11 C15:M24">
-    <cfRule type="cellIs" dxfId="37" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H10:M14 G12 F11 C15:M24">
-    <cfRule type="cellIs" dxfId="36" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="17" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N26">
-    <cfRule type="cellIs" dxfId="35" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="18" operator="greaterThan">
       <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N26">
-    <cfRule type="cellIs" dxfId="34" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="19" operator="equal">
       <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="33" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="20" operator="greaterThan">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="32" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="21" operator="equal">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="31" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="22" operator="greaterThan">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="30" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="23" operator="equal">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N3 N5:N8 N10:N16">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="greaterThan">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N3 N5:N8 N10:N16">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="cellIs" dxfId="27" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="cellIs" dxfId="26" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4 N9">
-    <cfRule type="cellIs" dxfId="19" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="47" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4 N9">
-    <cfRule type="cellIs" dxfId="18" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2930,7 +2970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -2999,10 +3039,10 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <v>0.16666666666666666</v>
       </c>
       <c r="C2" s="6">
@@ -3024,10 +3064,10 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C3" s="11">
@@ -3049,10 +3089,10 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="37">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C4" s="11">
@@ -3074,10 +3114,10 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>6.25E-2</v>
       </c>
       <c r="C5" s="11"/>
@@ -3099,10 +3139,10 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C6" s="11"/>
@@ -3124,10 +3164,10 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>0.10416666666666667</v>
       </c>
       <c r="C7" s="11"/>
@@ -3149,10 +3189,10 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C8" s="11"/>
@@ -3174,10 +3214,10 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>0.16666666666666666</v>
       </c>
       <c r="C9" s="13"/>
@@ -3199,10 +3239,10 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>0.10416666666666667</v>
       </c>
       <c r="C10" s="13"/>
@@ -3224,10 +3264,10 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="37">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C11" s="13"/>
@@ -3249,17 +3289,21 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="37">
         <v>0.10416666666666667</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="9"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="15"/>
+      <c r="F12" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H12" s="9"/>
       <c r="I12" s="13"/>
       <c r="J12" s="9"/>
@@ -3268,14 +3312,14 @@
       <c r="M12" s="12"/>
       <c r="N12" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>0.125</v>
       </c>
       <c r="C13" s="13"/>
@@ -3295,17 +3339,19 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="37">
         <v>0.10416666666666667</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="9"/>
       <c r="E14" s="11"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="11"/>
+      <c r="G14" s="11">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="H14" s="9"/>
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
@@ -3314,21 +3360,14 @@
       <c r="M14" s="12"/>
       <c r="N14" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="39">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="11"/>
+      <c r="A15" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="52"/>
       <c r="H15" s="9"/>
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
@@ -3341,21 +3380,15 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="39">
-        <v>1.25</v>
-      </c>
-      <c r="C16" s="11">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D16" s="9">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E16" s="11">
-        <v>9.0277777777777776E-2</v>
-      </c>
+      <c r="A16" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="37">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="9"/>
       <c r="G16" s="11"/>
       <c r="H16" s="9"/>
@@ -3365,23 +3398,29 @@
       <c r="L16" s="11"/>
       <c r="M16" s="12"/>
       <c r="N16" s="9">
-        <f t="shared" si="0"/>
-        <v>0.2361111111111111</v>
+        <f>SUM(H16:M16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="39">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C17" s="11"/>
+      <c r="A17" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="37">
+        <v>1.25</v>
+      </c>
+      <c r="C17" s="11">
+        <v>6.25E-2</v>
+      </c>
       <c r="D17" s="9">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="9"/>
+      <c r="E17" s="11">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0.125</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="9"/>
       <c r="I17" s="11"/>
@@ -3390,26 +3429,22 @@
       <c r="L17" s="11"/>
       <c r="M17" s="12"/>
       <c r="N17" s="9">
-        <f t="shared" si="0"/>
+        <f>SUM(H17:M17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="37">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="9">
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="39">
-        <v>0.1423611111111111</v>
-      </c>
-      <c r="C18" s="11">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="D18" s="11">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E18" s="11">
-        <v>1.7361111111111112E-2</v>
-      </c>
+      <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="11"/>
       <c r="H18" s="9"/>
@@ -3419,17 +3454,29 @@
       <c r="L18" s="11"/>
       <c r="M18" s="12"/>
       <c r="N18" s="9">
-        <f t="shared" si="0"/>
-        <v>3.8194444444444448E-2</v>
+        <f>SUM(H18:M18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="9"/>
+      <c r="A19" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="37">
+        <v>0.1423611111111111</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D19" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="9"/>
       <c r="I19" s="11"/>
@@ -3438,18 +3485,12 @@
       <c r="L19" s="11"/>
       <c r="M19" s="12"/>
       <c r="N19" s="9">
-        <f>SUM(C19:M19)</f>
+        <f>SUM(H19:M19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="11"/>
+      <c r="B20" s="52"/>
       <c r="H20" s="9"/>
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
@@ -3457,18 +3498,12 @@
       <c r="L20" s="11"/>
       <c r="M20" s="12"/>
       <c r="N20" s="9">
-        <f>SUM(C20:M20)</f>
+        <f>SUM(H20:M20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="B21" s="52"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -3476,18 +3511,12 @@
       <c r="L21" s="9"/>
       <c r="M21" s="12"/>
       <c r="N21" s="9">
-        <f>SUM(C21:M21)</f>
+        <f>SUM(H21:M21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="B22" s="52"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -3495,7 +3524,7 @@
       <c r="L22" s="11"/>
       <c r="M22" s="12"/>
       <c r="N22" s="9">
-        <f>SUM(C22:M22)</f>
+        <f>SUM(H22:M22)</f>
         <v>0</v>
       </c>
     </row>
@@ -3514,7 +3543,7 @@
       <c r="L23" s="11"/>
       <c r="M23" s="12"/>
       <c r="N23" s="9">
-        <f>SUM(C23:M23)</f>
+        <f t="shared" ref="N19:N24" si="1">SUM(C23:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -3533,7 +3562,7 @@
       <c r="L24" s="11"/>
       <c r="M24" s="12"/>
       <c r="N24" s="9">
-        <f>SUM(C24:M24)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3549,26 +3578,26 @@
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
-      <c r="M25" s="17"/>
+      <c r="M25" s="15"/>
       <c r="N25" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="23"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="21"/>
       <c r="N26" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3576,62 +3605,62 @@
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
-        <f t="shared" ref="B27:M27" si="1">SUM(B2:B26)</f>
+        <f t="shared" ref="B27:M27" si="2">SUM(B2:B26)</f>
         <v>3.6631944444444446</v>
       </c>
       <c r="C27" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34375</v>
       </c>
       <c r="D27" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34375</v>
       </c>
       <c r="E27" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="F27" s="9">
-        <f t="shared" si="1"/>
-        <v>0.13194444444444442</v>
+        <f t="shared" si="2"/>
+        <v>0.31597222222222215</v>
       </c>
       <c r="G27" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>9.722222222222221E-2</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H27" s="9">
-        <f t="shared" si="1"/>
+      <c r="I27" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I27" s="9">
-        <f t="shared" si="1"/>
+      <c r="J27" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="9">
-        <f t="shared" si="1"/>
+      <c r="K27" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K27" s="9">
-        <f t="shared" si="1"/>
+      <c r="L27" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L27" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="M27" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M28" s="9">
         <f>SUM(C27:M27)</f>
-        <v>1.1527777777777777</v>
+        <v>1.4340277777777777</v>
       </c>
       <c r="N28" s="9">
         <f>SUM(N2:N26)</f>
-        <v>1.1527777777777777</v>
+        <v>0.93402777777777779</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4605,84 +4634,104 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:M2 F22:F24 H22:I24 C20:C26 G20:G26 I20:I21 I25:I26 E20:E26 L20:L26 E3:E18 C3:C18 G3:G18 I3:I18 L3:L18">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 F23:F24 H22:I24 I20:I21 I25:I26 L20:L26 I3:I18 L3:L18 E3:E14 C3:C14 G3:G14 E23:E26 E16:E19 C23:C26 C16:C19 G23:G26 G16:G19">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M24">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M14 C23:M24 H15:M22 C16:G19">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19 I19 G19 E19 C19">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="L19 I19">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="H19:M19">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:K25 F25 H25 M25">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D24 G22:G24 J22:K24">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="D23:D24 G23:G24 J22:K24">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26 C25 E25:M25">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M24">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M14 C23:M24 H15:M22 C16:G19">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M24">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThan">
+  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M14 C23:M24 H15:M22 C16:G19">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N26">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="N2:N14 N23:N26">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N26">
-    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
+  <conditionalFormatting sqref="N2:N14 N23:N26">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="greaterThan">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="3" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="2" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="1" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="D19">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19:N22">
+    <cfRule type="cellIs" dxfId="3" priority="65" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19:N22">
+    <cfRule type="cellIs" dxfId="2" priority="68" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15:N18">
+    <cfRule type="cellIs" dxfId="1" priority="87" operator="greaterThan">
+      <formula>$B16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15:N18">
+    <cfRule type="cellIs" dxfId="0" priority="88" operator="equal">
+      <formula>$B16</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
fin du crud sur categorie
</commit_message>
<xml_diff>
--- a/annexes/Planification.xlsx
+++ b/annexes/Planification.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve">L'admin peut créer un utilisateur </t>
+  </si>
+  <si>
+    <t>ligne d'Arianne</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -477,11 +480,28 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="51">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD6E3BC"/>
+          <bgColor rgb="FFD6E3BC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBD4B4"/>
+          <bgColor rgb="FFFBD4B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2817,147 +2837,147 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F22:F24 H22:I24 C20:C26 G20:G26 I20:I26 E20:E26 L20:L26 D16:M16 H13:H14 G3:G9 E3:E5 C4:C18 I3:I18 L3:L18 E7:E18 G15:G18">
-    <cfRule type="cellIs" dxfId="48" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C20:M24 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H13:M14 G12:M12 H11:M11 F11 C15:M18">
-    <cfRule type="cellIs" dxfId="47" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19 I19 G19 E19 C19">
-    <cfRule type="cellIs" dxfId="46" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="11" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:M19">
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:K25 F25 H25 M25">
-    <cfRule type="cellIs" dxfId="44" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="13" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:D24 G22:G24 J22:K24">
-    <cfRule type="cellIs" dxfId="43" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="14" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 C4:M5 C7:M9 G6:M6 H10:M12 I13:M14 C15:M24">
-    <cfRule type="cellIs" dxfId="42" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H10:M14 G12 F11 C15:M24">
-    <cfRule type="cellIs" dxfId="41" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C26:M26 C25 E25:M25 E3:M3 C3 C4:M5 C7:M9 C6 F6:M6 C10:F10 C11:E12 C13:F14 H10:M14 G12 F11 C15:M24">
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="17" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N26">
-    <cfRule type="cellIs" dxfId="39" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="18" operator="greaterThan">
       <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N26">
-    <cfRule type="cellIs" dxfId="38" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="19" operator="equal">
       <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="37" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="20" operator="greaterThan">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="36" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="35" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="22" operator="greaterThan">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="34" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="23" operator="equal">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N3 N5:N8 N10:N16">
-    <cfRule type="cellIs" dxfId="33" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="27" operator="greaterThan">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N3 N5:N8 N10:N16">
-    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="32" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4 N9">
-    <cfRule type="cellIs" dxfId="23" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="47" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4 N9">
-    <cfRule type="cellIs" dxfId="22" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2968,10 +2988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3059,7 +3079,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9">
-        <f t="shared" ref="N2:N26" si="0">SUM(C2:M2)</f>
+        <f t="shared" ref="N2:N27" si="0">SUM(C2:M2)</f>
         <v>0.125</v>
       </c>
     </row>
@@ -3398,63 +3418,51 @@
       <c r="H16" s="9">
         <v>0.20833333333333334</v>
       </c>
-      <c r="I16" s="11"/>
+      <c r="I16" s="11">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="9">
-        <f t="shared" ref="N16:N22" si="1">SUM(H16:M16)</f>
-        <v>0.20833333333333334</v>
-      </c>
+      <c r="M16" s="53"/>
+      <c r="N16" s="9"/>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="37">
-        <v>1.25</v>
-      </c>
-      <c r="C17" s="11">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D17" s="9">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E17" s="11">
-        <v>9.0277777777777776E-2</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0.125</v>
-      </c>
-      <c r="G17" s="11">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="11"/>
+      <c r="A17" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="52"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="11"/>
       <c r="M17" s="12"/>
       <c r="N17" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="N17:N23" si="1">SUM(H17:M17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="37">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C18" s="11"/>
+        <v>1.25</v>
+      </c>
+      <c r="C18" s="11">
+        <v>6.25E-2</v>
+      </c>
       <c r="D18" s="9">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="11"/>
+      <c r="E18" s="11">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="H18" s="9"/>
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
@@ -3468,29 +3476,19 @@
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="37">
-        <v>0.1423611111111111</v>
-      </c>
-      <c r="C19" s="11">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="D19" s="11">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E19" s="11">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="F19" s="9">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="G19" s="11">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="H19" s="9">
-        <v>1.0416666666666666E-2</v>
-      </c>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="11"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -3498,29 +3496,53 @@
       <c r="M19" s="12"/>
       <c r="N19" s="9">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="37">
+        <v>0.1423611111111111</v>
+      </c>
+      <c r="C20" s="11">
         <v>1.0416666666666666E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="52"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="11"/>
+      <c r="D20" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="I20" s="11">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="11"/>
       <c r="M20" s="12"/>
       <c r="N20" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="52"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="I21" s="11"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
+      <c r="L21" s="11"/>
       <c r="M21" s="12"/>
       <c r="N21" s="9">
         <f t="shared" si="1"/>
@@ -3529,11 +3551,11 @@
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="52"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="12"/>
       <c r="N22" s="9">
         <f t="shared" si="1"/>
@@ -3541,13 +3563,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
+      <c r="B23" s="52"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -3555,7 +3571,7 @@
       <c r="L23" s="11"/>
       <c r="M23" s="12"/>
       <c r="N23" s="9">
-        <f t="shared" ref="N23:N24" si="2">SUM(C23:M23)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3574,7 +3590,7 @@
       <c r="L24" s="11"/>
       <c r="M24" s="12"/>
       <c r="N24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="N24:N25" si="2">SUM(C24:M24)</f>
         <v>0</v>
       </c>
     </row>
@@ -3582,6 +3598,7 @@
       <c r="A25" s="14"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -3590,92 +3607,109 @@
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
-      <c r="M25" s="15"/>
+      <c r="M25" s="12"/>
       <c r="N25" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="21"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="15"/>
       <c r="N26" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="9">
-        <f t="shared" ref="B27:M27" si="3">SUM(B2:B26)</f>
+      <c r="A27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="9">
+        <f t="shared" ref="B28:M28" si="3">SUM(B2:B27)</f>
         <v>3.6631944444444446</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C28" s="9">
         <f t="shared" si="3"/>
         <v>0.34375</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D28" s="9">
         <f t="shared" si="3"/>
         <v>0.34375</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E28" s="9">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F28" s="9">
         <f t="shared" si="3"/>
         <v>0.31597222222222215</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G28" s="9">
         <f t="shared" si="3"/>
         <v>0.28124999999999994</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H28" s="9">
         <f t="shared" si="3"/>
         <v>0.34375000000000006</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I28" s="9">
+        <f t="shared" si="3"/>
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="J28" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J27" s="9">
+      <c r="K28" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K27" s="9">
+      <c r="L28" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L27" s="9">
+      <c r="M28" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M27" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M28" s="9">
-        <f>SUM(C27:M27)</f>
-        <v>1.9618055555555554</v>
-      </c>
-      <c r="N28" s="9">
-        <f>SUM(N2:N26)</f>
-        <v>1.2777777777777779</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="9">
+        <f>SUM(C28:M28)</f>
+        <v>2.270833333333333</v>
+      </c>
+      <c r="N29" s="9">
+        <f>SUM(N2:N27)</f>
+        <v>1.0868055555555556</v>
+      </c>
+    </row>
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4645,105 +4679,116 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:M2 F23:F24 H22:I24 I20:I21 I25:I26 L20:L26 I3:I18 L3:L18 E3:E14 C3:C14 G3:G14 E23:E26 E16:E19 C23:C26 C16:C19 G23:G26 G16:G19">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 F24:F25 H23:I25 I21:I22 I26:I27 L21:L27 L3:L19 E3:E14 C3:C14 G3:G14 E24:E27 C24:C27 G24:G27 E18:E20 E16 C18:C20 C16 G18:G20 G16 I18:I19 I3:I16">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M14 C23:M24 H15:M22 C16:G19">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M14 C24:M25 H15:M15 C18:G20 H18:M23 J17:M17 C16:M16">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19 I19">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="L20 I20">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19:M19">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="H20:M20">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J25:K25 F25 H25 M25">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="J26:K26 F26 H26 M26">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23:D24 G23:G24 J22:K24">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="D24:D25 G24:G25 J23:K25">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:M26 C25 E25:M25">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27 C26 E26:M26">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M14 C23:M24 H15:M22 C16:G19">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M14 C24:M25 H15:M15 C18:G20 H18:M23 J17:M17 C16:M16">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:M26 C25 E25:M25 C2:M14 C23:M24 H15:M22 C16:G19">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
+  <conditionalFormatting sqref="C27:M27 C26 E26:M26 C2:M14 C24:M25 H15:M15 C18:G20 H18:M23 J17:M17 C16:M16">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N14 N23:N26">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="N2:N14 N24:N27">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N14 N23:N26">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+  <conditionalFormatting sqref="N2:N14 N24:N27">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="B28">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="greaterThan">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+  <conditionalFormatting sqref="B28">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>3.666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="C28:M28">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="greaterThan">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+  <conditionalFormatting sqref="C28:M28">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
       <formula>0.3333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="D20">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N19:N22">
-    <cfRule type="cellIs" dxfId="3" priority="65" operator="greaterThan">
+  <conditionalFormatting sqref="N20:N23">
+    <cfRule type="cellIs" dxfId="5" priority="65" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N19:N22">
-    <cfRule type="cellIs" dxfId="2" priority="68" operator="equal">
+  <conditionalFormatting sqref="N20:N23">
+    <cfRule type="cellIs" dxfId="4" priority="68" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N15:N18">
-    <cfRule type="cellIs" dxfId="1" priority="87" operator="greaterThan">
+  <conditionalFormatting sqref="N17:N19 N15">
+    <cfRule type="cellIs" dxfId="3" priority="87" operator="greaterThan">
       <formula>$B16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N15:N18">
-    <cfRule type="cellIs" dxfId="0" priority="88" operator="equal">
+  <conditionalFormatting sqref="N17:N19 N15">
+    <cfRule type="cellIs" dxfId="2" priority="88" operator="equal">
       <formula>$B16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16">
+    <cfRule type="cellIs" dxfId="1" priority="89" operator="greaterThan">
+      <formula>$B18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16">
+    <cfRule type="cellIs" dxfId="0" priority="91" operator="equal">
+      <formula>$B18</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
avancement de la doc + avancement des test + correction de quelques bugs
</commit_message>
<xml_diff>
--- a/annexes/Planification.xlsx
+++ b/annexes/Planification.xlsx
@@ -2991,7 +2991,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3467,13 +3467,15 @@
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="11"/>
-      <c r="J18" s="9"/>
+      <c r="J18" s="9">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="K18" s="9"/>
       <c r="L18" s="11"/>
       <c r="M18" s="12"/>
       <c r="N18" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3492,13 +3494,15 @@
       <c r="G19" s="11"/>
       <c r="H19" s="9"/>
       <c r="I19" s="11"/>
-      <c r="J19" s="9"/>
+      <c r="J19" s="9">
+        <v>0.125</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="L19" s="11"/>
       <c r="M19" s="12"/>
       <c r="N19" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3529,13 +3533,15 @@
       <c r="I20" s="11">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="J20" s="9"/>
+      <c r="J20" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="K20" s="9"/>
       <c r="L20" s="11"/>
       <c r="M20" s="12"/>
       <c r="N20" s="9">
         <f t="shared" si="1"/>
-        <v>2.7777777777777776E-2</v>
+        <v>3.8194444444444441E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3687,7 +3693,7 @@
       </c>
       <c r="J28" s="9">
         <f t="shared" si="3"/>
-        <v>6.25E-2</v>
+        <v>0.34375000000000006</v>
       </c>
       <c r="K28" s="9">
         <f t="shared" si="3"/>
@@ -3705,11 +3711,11 @@
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M29" s="9">
         <f>SUM(C28:M28)</f>
-        <v>2.333333333333333</v>
+        <v>2.614583333333333</v>
       </c>
       <c r="N29" s="9">
         <f>SUM(N2:N27)</f>
-        <v>1.1493055555555556</v>
+        <v>1.4305555555555556</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ajout du manuel utilisateur + correction de bug
</commit_message>
<xml_diff>
--- a/annexes/Planification.xlsx
+++ b/annexes/Planification.xlsx
@@ -2991,7 +2991,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3470,12 +3470,14 @@
       <c r="J18" s="9">
         <v>0.14583333333333334</v>
       </c>
-      <c r="K18" s="9"/>
+      <c r="K18" s="9">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="L18" s="11"/>
       <c r="M18" s="12"/>
       <c r="N18" s="9">
         <f t="shared" si="1"/>
-        <v>0.14583333333333334</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3497,12 +3499,14 @@
       <c r="J19" s="9">
         <v>0.125</v>
       </c>
-      <c r="K19" s="9"/>
+      <c r="K19" s="9">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="L19" s="11"/>
       <c r="M19" s="12"/>
       <c r="N19" s="9">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>0.29166666666666663</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3536,12 +3540,14 @@
       <c r="J20" s="9">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="K20" s="9"/>
+      <c r="K20" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="L20" s="11"/>
       <c r="M20" s="12"/>
       <c r="N20" s="9">
         <f t="shared" si="1"/>
-        <v>3.8194444444444441E-2</v>
+        <v>4.8611111111111105E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3697,7 +3703,7 @@
       </c>
       <c r="K28" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.34375</v>
       </c>
       <c r="L28" s="9">
         <f t="shared" si="3"/>
@@ -3711,11 +3717,11 @@
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M29" s="9">
         <f>SUM(C28:M28)</f>
-        <v>2.614583333333333</v>
+        <v>2.958333333333333</v>
       </c>
       <c r="N29" s="9">
         <f>SUM(N2:N27)</f>
-        <v>1.4305555555555556</v>
+        <v>1.7743055555555558</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>